<commit_message>
export to xml and csv is done
</commit_message>
<xml_diff>
--- a/public/exports/csv/books.xlsx
+++ b/public/exports/csv/books.xlsx
@@ -15,12 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t>Book Title</t>
-  </si>
-  <si>
-    <t>Uncle Pop</t>
   </si>
   <si>
     <t>Test</t>
@@ -362,7 +359,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -370,19 +367,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
exporting xml and csv files
</commit_message>
<xml_diff>
--- a/public/exports/csv/books.xlsx
+++ b/public/exports/csv/books.xlsx
@@ -15,14 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
-  <si>
-    <t>Book Title</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,25 +352,14 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>